<commit_message>
edits to new sections at bottom, MoTM Schedule, Top Scorers of Week, Full Table
</commit_message>
<xml_diff>
--- a/data/motm_schedule.xlsx
+++ b/data/motm_schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/238205feaa974794/Desktop/Rangolytics/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0804E9C3-EE08-4622-A80E-57189EF86C44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="8_{0804E9C3-EE08-4622-A80E-57189EF86C44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD6C4B25-860A-4856-8BCC-6FA0F89A4961}"/>
   <bookViews>
     <workbookView xWindow="6645" yWindow="6060" windowWidth="21600" windowHeight="11385" xr2:uid="{DDF0D80A-BED2-46DC-88A3-238DA66DB172}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
   <si>
     <t>MoTM</t>
   </si>
@@ -153,6 +153,33 @@
   </si>
   <si>
     <t>GW 38</t>
+  </si>
+  <si>
+    <t>Winner</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>Momoney</t>
+  </si>
+  <si>
+    <t>Gabi-Gabi-Gabagool</t>
+  </si>
+  <si>
+    <t>Minnows FC</t>
+  </si>
+  <si>
+    <t>Saka Souffle</t>
+  </si>
+  <si>
+    <t>Berba Juniors</t>
+  </si>
+  <si>
+    <t>MB FC</t>
+  </si>
+  <si>
+    <t>ChicagoFire</t>
   </si>
 </sst>
 </file>
@@ -527,222 +554,259 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DDA8A60-0423-4089-A128-E830C37C5432}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F3" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F4" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="1">
+      <c r="F5" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F6" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F7" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="1">
+      <c r="F8" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="1">
+      <c r="F9" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="1">
+      <c r="F10" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="1">
+      <c r="F11" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="1">
+      <c r="F12" s="1">
         <v>3</v>
       </c>
     </row>

</xml_diff>